<commit_message>
5, 12, 139, 189, 227, 238, 300, 415, 468, 523, 621, 674, 825, 863, 896, 921, 977, 1143
</commit_message>
<xml_diff>
--- a/面试题汇总/Facebook面经题汇总-最新整理.xlsx
+++ b/面试题汇总/Facebook面经题汇总-最新整理.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hjj/Desktop/HJJ/LeetCode/面试题汇总/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C47EC-CE5D-6545-A529-CCCFA03EDEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9297EA-AA3A-F64D-A170-BF7824514DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>418 · 整数转罗马数字</t>
   </si>
   <si>
-    <t>780 · 删除无效的括号</t>
-  </si>
-  <si>
     <t>669 · 换硬币</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>838 · 子数组和为K</t>
   </si>
   <si>
-    <t>945 · 任务计划</t>
-  </si>
-  <si>
     <t>1115 · 二叉树每层的平均数</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>1393 · 适龄的朋友</t>
   </si>
   <si>
-    <t>1465 · 任务顺序</t>
-  </si>
-  <si>
     <t>1506 · 二叉树中所有距离为 K 的结点</t>
   </si>
   <si>
@@ -301,9 +292,6 @@
   </si>
   <si>
     <t>https://www.lintcode.com/problem/200/?utm_source=sc-libao-zyq</t>
-  </si>
-  <si>
-    <t>154 · 正则表达式匹配</t>
   </si>
   <si>
     <t>https://www.lintcode.com/problem/154/?utm_source=sc-libao-zyq</t>
@@ -1728,6 +1716,18 @@
   </si>
   <si>
     <t>606 · 第K大的元素 II (无此题)</t>
+  </si>
+  <si>
+    <t>780 · 删除无效的括号 (hard)</t>
+  </si>
+  <si>
+    <t>154 · 正则表达式匹配 (hard)</t>
+  </si>
+  <si>
+    <t>945 · 任务计划</t>
+  </si>
+  <si>
+    <t>1465 · 任务顺序 (无此题)</t>
   </si>
 </sst>
 </file>
@@ -2313,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="125" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="66" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14"/>
@@ -2325,7 +2325,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="44" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
@@ -2336,144 +2336,144 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="7"/>
       <c r="B5" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16">
       <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
       <c r="A8" s="14"/>
       <c r="B8" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
       <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16">
       <c r="A12" s="14"/>
       <c r="B12" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16">
       <c r="A14" s="14"/>
       <c r="B14" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16">
       <c r="A15" s="14"/>
       <c r="B15" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16">
       <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16">
       <c r="A17" s="14"/>
       <c r="B17" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16">
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16">
@@ -2491,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16">
@@ -2500,16 +2500,16 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16">
       <c r="A21" s="14"/>
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16">
@@ -2518,7 +2518,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16">
@@ -2527,7 +2527,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16">
@@ -2536,7 +2536,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16">
@@ -2545,25 +2545,25 @@
         <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16">
       <c r="A26" s="14"/>
       <c r="B26" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16">
       <c r="A27" s="14"/>
       <c r="B27" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16">
@@ -2572,7 +2572,7 @@
         <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
@@ -2581,16 +2581,16 @@
         <v>35</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16">
       <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16">
@@ -2599,34 +2599,34 @@
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16">
       <c r="A32" s="14"/>
       <c r="B32" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16">
       <c r="A33" s="14"/>
       <c r="B33" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16">
       <c r="A34" s="14"/>
       <c r="B34" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16">
@@ -2635,16 +2635,16 @@
         <v>16</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16">
       <c r="A36" s="14"/>
       <c r="B36" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16">
@@ -2653,18 +2653,18 @@
         <v>23</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16">
       <c r="A38" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16">
@@ -2673,7 +2673,7 @@
         <v>9</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16">
@@ -2682,7 +2682,7 @@
         <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16">
@@ -2691,7 +2691,7 @@
         <v>11</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16">
@@ -2700,7 +2700,7 @@
         <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16">
@@ -2709,7 +2709,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16">
@@ -2718,7 +2718,7 @@
         <v>14</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16">
@@ -2727,7 +2727,7 @@
         <v>15</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16">
@@ -2736,7 +2736,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16">
@@ -2745,7 +2745,7 @@
         <v>18</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16">
@@ -2754,16 +2754,16 @@
         <v>19</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="16">
       <c r="A49" s="17"/>
       <c r="B49" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="16">
@@ -2772,25 +2772,25 @@
         <v>20</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="16">
       <c r="A51" s="17"/>
       <c r="B51" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16">
       <c r="A52" s="17"/>
       <c r="B52" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16">
@@ -2799,7 +2799,7 @@
         <v>21</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16">
@@ -2808,25 +2808,25 @@
         <v>22</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16">
       <c r="A55" s="17"/>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="16">
       <c r="A56" s="17"/>
       <c r="B56" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="16">
@@ -2835,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16">
@@ -2844,7 +2844,7 @@
         <v>26</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="16">
@@ -2853,7 +2853,7 @@
         <v>27</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="16">
@@ -2862,7 +2862,7 @@
         <v>29</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="16">
@@ -2871,7 +2871,7 @@
         <v>30</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="16">
@@ -2880,7 +2880,7 @@
         <v>31</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="16">
@@ -2889,43 +2889,43 @@
         <v>32</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="16">
       <c r="A64" s="17"/>
       <c r="B64" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16">
       <c r="A65" s="17"/>
       <c r="B65" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16">
       <c r="A66" s="17"/>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="16">
       <c r="A67" s="17"/>
       <c r="B67" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="16">
@@ -2934,7 +2934,7 @@
         <v>36</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="16">
@@ -2943,16 +2943,16 @@
         <v>37</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="16">
       <c r="A70" s="17"/>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="16">
@@ -2961,133 +2961,133 @@
         <v>39</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="16">
       <c r="A72" s="17"/>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16">
       <c r="A73" s="17"/>
       <c r="B73" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16">
       <c r="A74" s="17"/>
       <c r="B74" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16">
       <c r="A75" s="17"/>
       <c r="B75" s="4" t="s">
-        <v>41</v>
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16">
       <c r="A76" s="17"/>
       <c r="B76" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16">
       <c r="A77" s="17"/>
       <c r="B77" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="16">
       <c r="A78" s="17"/>
       <c r="B78" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="16">
       <c r="A79" s="17"/>
       <c r="B79" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="16">
       <c r="A80" s="17"/>
       <c r="B80" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="16">
       <c r="A81" s="17"/>
       <c r="B81" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="16">
       <c r="A82" s="17"/>
       <c r="B82" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="16">
       <c r="A83" s="17"/>
-      <c r="B83" s="4" t="s">
-        <v>48</v>
+      <c r="B83" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="16">
       <c r="A84" s="17"/>
       <c r="B84" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="16">
       <c r="A85" s="17"/>
-      <c r="B85" s="4" t="s">
-        <v>49</v>
+      <c r="B85" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="16">
@@ -3096,349 +3096,349 @@
         <v>37</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="16">
       <c r="A87" s="17"/>
       <c r="B87" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="16">
       <c r="A88" s="17"/>
       <c r="B88" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="16">
       <c r="A89" s="17"/>
-      <c r="B89" s="4" t="s">
-        <v>54</v>
+      <c r="B89" s="9" t="s">
+        <v>239</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="16">
       <c r="A90" s="17"/>
       <c r="B90" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="16">
       <c r="A91" s="17"/>
-      <c r="B91" s="4" t="s">
-        <v>56</v>
+      <c r="B91" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="16">
       <c r="A92" s="17"/>
       <c r="B92" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="16">
       <c r="A93" s="17"/>
       <c r="B93" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="16">
       <c r="A94" s="17"/>
       <c r="B94" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="16">
       <c r="A95" s="17"/>
       <c r="B95" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="16">
       <c r="A96" s="17"/>
-      <c r="B96" s="4" t="s">
-        <v>60</v>
+      <c r="B96" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="16">
       <c r="A97" s="17"/>
       <c r="B97" s="4" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="16">
       <c r="A98" s="16"/>
       <c r="B98" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="16">
       <c r="A99" s="17"/>
-      <c r="B99" s="4" t="s">
-        <v>63</v>
+      <c r="B99" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="16">
       <c r="A100" s="17"/>
       <c r="B100" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="16">
       <c r="A101" s="17"/>
-      <c r="B101" s="1" t="s">
-        <v>65</v>
+      <c r="B101" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="16">
       <c r="A102" s="17"/>
       <c r="B102" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="16">
       <c r="A103" s="17"/>
       <c r="B103" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="16">
       <c r="A104" s="17"/>
       <c r="B104" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="16">
       <c r="A105" s="17"/>
       <c r="B105" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="16">
       <c r="A106" s="17"/>
       <c r="B106" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="16">
       <c r="A107" s="17"/>
-      <c r="B107" s="1" t="s">
-        <v>70</v>
+      <c r="B107" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="16">
       <c r="A108" s="17"/>
       <c r="B108" s="1" t="s">
-        <v>71</v>
+        <v>240</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="16">
       <c r="A109" s="17"/>
-      <c r="B109" s="1" t="s">
-        <v>72</v>
+      <c r="B109" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="16">
       <c r="A110" s="17"/>
       <c r="B110" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="16">
       <c r="A111" s="17"/>
       <c r="B111" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="16">
       <c r="A112" s="17"/>
-      <c r="B112" s="1" t="s">
-        <v>56</v>
+      <c r="B112" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="16">
       <c r="A113" s="17"/>
       <c r="B113" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="16">
       <c r="A114" s="17"/>
       <c r="B114" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="16">
       <c r="A115" s="17"/>
-      <c r="B115" s="4" t="s">
-        <v>77</v>
+      <c r="B115" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="16">
       <c r="A116" s="17"/>
-      <c r="B116" s="1" t="s">
-        <v>78</v>
+      <c r="B116" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="16">
       <c r="A117" s="17"/>
       <c r="B117" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="16">
       <c r="A118" s="17"/>
       <c r="B118" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="16">
       <c r="A119" s="17"/>
-      <c r="B119" s="1" t="s">
-        <v>87</v>
+      <c r="B119" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="16">
       <c r="A120" s="17"/>
       <c r="B120" s="1" t="s">
-        <v>89</v>
+        <v>238</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="16">
       <c r="A121" s="17"/>
       <c r="B121" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="16">
       <c r="A122" s="17"/>
       <c r="B122" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="16">
       <c r="A123" s="17"/>
       <c r="B123" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="16">
       <c r="A124" s="17"/>
       <c r="B124" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>